<commit_message>
fish all code and it's work
</commit_message>
<xml_diff>
--- a/Spec_mul.xlsx
+++ b/Spec_mul.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8475" activeTab="3"/>
+    <workbookView windowWidth="20385" windowHeight="8580" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HP 974A" sheetId="16" r:id="rId1"/>
     <sheet name="Keysight U1253B" sheetId="18" r:id="rId2"/>
     <sheet name="Fluke 189" sheetId="19" r:id="rId3"/>
     <sheet name="Agilent 34401A" sheetId="20" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="21" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525" fullCalcOnLoad="true" concurrentCalc="false"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="19">
   <si>
     <t>meas_type</t>
   </si>
@@ -60,21 +61,36 @@
   <si>
     <t>Iac_45_1000</t>
   </si>
+  <si>
+    <t>x_</t>
+  </si>
+  <si>
+    <t>U_G_</t>
+  </si>
+  <si>
+    <t>U_FS_</t>
+  </si>
+  <si>
+    <t>U_</t>
+  </si>
+  <si>
+    <t>u_</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="##0E+0"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="##0.000E+0"/>
-    <numFmt numFmtId="178" formatCode="0.0000"/>
+    <numFmt numFmtId="176" formatCode="##0.000E+0"/>
+    <numFmt numFmtId="177" formatCode="##0E+0"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="0.0000"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,9 +108,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -106,8 +182,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -115,21 +207,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -145,15 +222,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,38 +236,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,38 +250,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="40">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,7 +302,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519242"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519242"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519242"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.5999938962981"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.5999938962981"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519242"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519242"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,31 +410,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.79998168889431"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.79998168889431"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,103 +452,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,36 +464,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.79998168889431"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="21">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -623,39 +620,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -667,17 +631,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -706,6 +659,50 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.49998474074526"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -720,279 +717,287 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="20" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="19" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="14" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="178" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="178" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="178" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="178" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="177" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accento6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accento6" xfId="2" builtinId="51"/>
+    <cellStyle name="20% - Accento6" xfId="3" builtinId="50"/>
+    <cellStyle name="Verifica Cella" xfId="4" builtinId="23"/>
+    <cellStyle name="Non Valido" xfId="5" builtinId="27"/>
+    <cellStyle name="40% - Accento5" xfId="6" builtinId="47"/>
+    <cellStyle name="Neutrale" xfId="7" builtinId="28"/>
+    <cellStyle name="40% - Accento4" xfId="8" builtinId="43"/>
+    <cellStyle name="20% - Accento4" xfId="9" builtinId="42"/>
+    <cellStyle name="40% - Accento3" xfId="10" builtinId="39"/>
+    <cellStyle name="20% - Accento3" xfId="11" builtinId="38"/>
+    <cellStyle name="60% - Accento2" xfId="12" builtinId="36"/>
+    <cellStyle name="Calcolo" xfId="13" builtinId="22"/>
+    <cellStyle name="40% - Accento2" xfId="14" builtinId="35"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10"/>
+    <cellStyle name="20% - Accento2" xfId="16" builtinId="34"/>
+    <cellStyle name="60% - Accento1" xfId="17" builtinId="32"/>
+    <cellStyle name="20% - Accento1" xfId="18" builtinId="30"/>
+    <cellStyle name="Buono" xfId="19" builtinId="26"/>
+    <cellStyle name="Cella Collegata" xfId="20" builtinId="24"/>
+    <cellStyle name="Accento6" xfId="21" builtinId="49"/>
+    <cellStyle name="40% - Accento1" xfId="22" builtinId="31"/>
+    <cellStyle name="Titolo 4" xfId="23" builtinId="19"/>
+    <cellStyle name="Accento5" xfId="24" builtinId="45"/>
+    <cellStyle name="Titolo 1" xfId="25" builtinId="16"/>
+    <cellStyle name="Testo Avviso" xfId="26" builtinId="11"/>
+    <cellStyle name="Titolo 3" xfId="27" builtinId="18"/>
+    <cellStyle name="Testo Esplicativo" xfId="28" builtinId="53"/>
+    <cellStyle name="Accento4" xfId="29" builtinId="41"/>
+    <cellStyle name="Titolo 2" xfId="30" builtinId="17"/>
+    <cellStyle name="20% - Accento5" xfId="31" builtinId="46"/>
+    <cellStyle name="Collegamento Ipertestuale" xfId="32" builtinId="8"/>
+    <cellStyle name="60% - Accento3" xfId="33" builtinId="40"/>
+    <cellStyle name="Currency [0]" xfId="34" builtinId="7"/>
+    <cellStyle name="60% - Accento4" xfId="35" builtinId="44"/>
+    <cellStyle name="Accento1" xfId="36" builtinId="29"/>
+    <cellStyle name="Totale" xfId="37" builtinId="25"/>
+    <cellStyle name="Collegamento Ipertestuale Seguito" xfId="38" builtinId="9"/>
+    <cellStyle name="Comma [0]" xfId="39" builtinId="6"/>
+    <cellStyle name="Accento3" xfId="40" builtinId="37"/>
+    <cellStyle name="60% - Accento5" xfId="41" builtinId="48"/>
+    <cellStyle name="Moneta" xfId="42" builtinId="4"/>
+    <cellStyle name="Output" xfId="43" builtinId="21"/>
+    <cellStyle name="Titolo" xfId="44" builtinId="15"/>
+    <cellStyle name="Input" xfId="45" builtinId="20"/>
+    <cellStyle name="Percentuale" xfId="46" builtinId="5"/>
+    <cellStyle name="Accento2" xfId="47" builtinId="33"/>
+    <cellStyle name="Virgola" xfId="48" builtinId="3"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1267,13 +1272,13 @@
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.8333333333333" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="11.8333333333333" customWidth="1"/>
-    <col min="2" max="5" width="10.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="11.833333333333" customWidth="true"/>
+    <col min="2" max="5" width="10.666666666667" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2">
       <c r="A2" s="40" t="s">
         <v>5</v>
       </c>
@@ -1307,7 +1312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3">
       <c r="A3" s="32" t="s">
         <v>5</v>
       </c>
@@ -1324,7 +1329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4">
       <c r="A4" s="40" t="s">
         <v>5</v>
       </c>
@@ -1341,7 +1346,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5">
       <c r="A5" s="32" t="s">
         <v>5</v>
       </c>
@@ -1358,7 +1363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6">
       <c r="A6" s="28" t="s">
         <v>5</v>
       </c>
@@ -1375,7 +1380,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7">
       <c r="A7" s="43" t="s">
         <v>6</v>
       </c>
@@ -1392,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8">
       <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
@@ -1409,7 +1414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9">
       <c r="A9" s="43" t="s">
         <v>6</v>
       </c>
@@ -1426,7 +1431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10">
       <c r="A10" s="63" t="s">
         <v>6</v>
       </c>
@@ -1443,7 +1448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11">
       <c r="A11" s="40" t="s">
         <v>7</v>
       </c>
@@ -1460,7 +1465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12">
       <c r="A12" s="32" t="s">
         <v>7</v>
       </c>
@@ -1477,7 +1482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13">
       <c r="A13" s="40" t="s">
         <v>7</v>
       </c>
@@ -1494,7 +1499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14">
       <c r="A14" s="32" t="s">
         <v>7</v>
       </c>
@@ -1511,7 +1516,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15">
       <c r="A15" s="40" t="s">
         <v>7</v>
       </c>
@@ -1528,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16">
       <c r="A16" s="52" t="s">
         <v>7</v>
       </c>
@@ -1545,7 +1550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17">
       <c r="A17" s="43" t="s">
         <v>8</v>
       </c>
@@ -1562,7 +1567,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18">
       <c r="A18" s="46" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +1584,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19">
       <c r="A19" s="43" t="s">
         <v>8</v>
       </c>
@@ -1596,7 +1601,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20">
       <c r="A20" s="46" t="s">
         <v>8</v>
       </c>
@@ -1613,7 +1618,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21">
       <c r="A21" s="49" t="s">
         <v>8</v>
       </c>
@@ -1630,7 +1635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22">
       <c r="A22" s="40" t="s">
         <v>9</v>
       </c>
@@ -1647,7 +1652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23">
       <c r="A23" s="32" t="s">
         <v>9</v>
       </c>
@@ -1664,7 +1669,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24">
       <c r="A24" s="40" t="s">
         <v>9</v>
       </c>
@@ -1681,7 +1686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25">
       <c r="A25" s="52" t="s">
         <v>9</v>
       </c>
@@ -1711,16 +1716,16 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.8333333333333" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="11.8333333333333" customWidth="1"/>
-    <col min="2" max="5" width="10.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="11.833333333333" customWidth="true"/>
+    <col min="2" max="5" width="10.666666666667" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -1737,7 +1742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2">
       <c r="A2" s="40" t="s">
         <v>5</v>
       </c>
@@ -1754,7 +1759,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3">
       <c r="A3" s="32" t="s">
         <v>5</v>
       </c>
@@ -1771,7 +1776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4">
       <c r="A4" s="40" t="s">
         <v>5</v>
       </c>
@@ -1788,7 +1793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5">
       <c r="A5" s="32" t="s">
         <v>5</v>
       </c>
@@ -1805,7 +1810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6">
       <c r="A6" s="40" t="s">
         <v>5</v>
       </c>
@@ -1822,7 +1827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7">
       <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
@@ -1839,7 +1844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8">
       <c r="A8" s="28" t="s">
         <v>5</v>
       </c>
@@ -1856,7 +1861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9">
       <c r="A9" s="43" t="s">
         <v>7</v>
       </c>
@@ -1873,7 +1878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10">
       <c r="A10" s="46" t="s">
         <v>7</v>
       </c>
@@ -1890,7 +1895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11">
       <c r="A11" s="43" t="s">
         <v>7</v>
       </c>
@@ -1907,7 +1912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12">
       <c r="A12" s="46" t="s">
         <v>7</v>
       </c>
@@ -1924,7 +1929,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13">
       <c r="A13" s="43" t="s">
         <v>7</v>
       </c>
@@ -1941,7 +1946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14">
       <c r="A14" s="46" t="s">
         <v>7</v>
       </c>
@@ -1958,7 +1963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15">
       <c r="A15" s="49" t="s">
         <v>7</v>
       </c>
@@ -1975,7 +1980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16">
       <c r="A16" s="40" t="s">
         <v>6</v>
       </c>
@@ -1992,7 +1997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17">
       <c r="A17" s="32" t="s">
         <v>6</v>
       </c>
@@ -2009,7 +2014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18">
       <c r="A18" s="40" t="s">
         <v>6</v>
       </c>
@@ -2026,7 +2031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19">
       <c r="A19" s="32" t="s">
         <v>6</v>
       </c>
@@ -2043,7 +2048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20">
       <c r="A20" s="40" t="s">
         <v>6</v>
       </c>
@@ -2060,7 +2065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21">
       <c r="A21" s="52" t="s">
         <v>6</v>
       </c>
@@ -2077,7 +2082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22">
       <c r="A22" s="43" t="s">
         <v>10</v>
       </c>
@@ -2094,7 +2099,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23">
       <c r="A23" s="46" t="s">
         <v>10</v>
       </c>
@@ -2111,7 +2116,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24">
       <c r="A24" s="43" t="s">
         <v>10</v>
       </c>
@@ -2128,7 +2133,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25">
       <c r="A25" s="46" t="s">
         <v>10</v>
       </c>
@@ -2145,7 +2150,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26">
       <c r="A26" s="43" t="s">
         <v>10</v>
       </c>
@@ -2162,7 +2167,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27">
       <c r="A27" s="46" t="s">
         <v>10</v>
       </c>
@@ -2179,7 +2184,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28">
       <c r="A28" s="49" t="s">
         <v>10</v>
       </c>
@@ -2196,7 +2201,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29">
       <c r="A29" s="40" t="s">
         <v>11</v>
       </c>
@@ -2213,7 +2218,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30">
       <c r="A30" s="32" t="s">
         <v>11</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31">
       <c r="A31" s="40" t="s">
         <v>11</v>
       </c>
@@ -2247,7 +2252,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32">
       <c r="A32" s="32" t="s">
         <v>11</v>
       </c>
@@ -2264,7 +2269,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33">
       <c r="A33" s="40" t="s">
         <v>11</v>
       </c>
@@ -2281,7 +2286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34">
       <c r="A34" s="52" t="s">
         <v>11</v>
       </c>
@@ -2311,17 +2316,17 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:I6"/>
+      <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.8333333333333" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="11.8333333333333" customWidth="1"/>
-    <col min="2" max="5" width="10.6666666666667" customWidth="1"/>
-    <col min="7" max="7" width="9.83333333333333" customWidth="1"/>
+    <col min="1" max="1" width="11.833333333333" customWidth="true"/>
+    <col min="2" max="5" width="10.666666666667" customWidth="true"/>
+    <col min="7" max="7" width="9.8333333333333" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1">
       <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
@@ -2338,7 +2343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2">
       <c r="A2" s="40" t="s">
         <v>5</v>
       </c>
@@ -2355,7 +2360,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3">
       <c r="A3" s="32" t="s">
         <v>5</v>
       </c>
@@ -2372,7 +2377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4">
       <c r="A4" s="40" t="s">
         <v>5</v>
       </c>
@@ -2389,7 +2394,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5">
       <c r="A5" s="32" t="s">
         <v>5</v>
       </c>
@@ -2406,7 +2411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6">
       <c r="A6" s="40" t="s">
         <v>5</v>
       </c>
@@ -2423,7 +2428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7">
       <c r="A7" s="32" t="s">
         <v>5</v>
       </c>
@@ -2440,7 +2445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8">
       <c r="A8" s="28" t="s">
         <v>5</v>
       </c>
@@ -2457,7 +2462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9">
       <c r="A9" s="43" t="s">
         <v>7</v>
       </c>
@@ -2474,7 +2479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10">
       <c r="A10" s="46" t="s">
         <v>7</v>
       </c>
@@ -2491,7 +2496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11">
       <c r="A11" s="43" t="s">
         <v>7</v>
       </c>
@@ -2508,7 +2513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12">
       <c r="A12" s="46" t="s">
         <v>7</v>
       </c>
@@ -2525,7 +2530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13">
       <c r="A13" s="43" t="s">
         <v>7</v>
       </c>
@@ -2542,7 +2547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14">
       <c r="A14" s="43" t="s">
         <v>7</v>
       </c>
@@ -2559,7 +2564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15">
       <c r="A15" s="46" t="s">
         <v>7</v>
       </c>
@@ -2576,7 +2581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16">
       <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
@@ -2593,7 +2598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17">
       <c r="A17" s="49" t="s">
         <v>7</v>
       </c>
@@ -2610,7 +2615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18">
       <c r="A18" s="40" t="s">
         <v>6</v>
       </c>
@@ -2627,7 +2632,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19">
       <c r="A19" s="32" t="s">
         <v>6</v>
       </c>
@@ -2644,7 +2649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20">
       <c r="A20" s="40" t="s">
         <v>6</v>
       </c>
@@ -2661,7 +2666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21">
       <c r="A21" s="32" t="s">
         <v>6</v>
       </c>
@@ -2678,7 +2683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22">
       <c r="A22" s="40" t="s">
         <v>6</v>
       </c>
@@ -2695,7 +2700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23">
       <c r="A23" s="52" t="s">
         <v>6</v>
       </c>
@@ -2712,7 +2717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24">
       <c r="A24" s="43" t="s">
         <v>12</v>
       </c>
@@ -2729,7 +2734,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25">
       <c r="A25" s="43" t="s">
         <v>12</v>
       </c>
@@ -2738,7 +2743,7 @@
       <c r="D25" s="48"/>
       <c r="E25" s="60"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26">
       <c r="A26" s="43" t="s">
         <v>12</v>
       </c>
@@ -2747,7 +2752,7 @@
       <c r="D26" s="45"/>
       <c r="E26" s="59"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27">
       <c r="A27" s="43" t="s">
         <v>12</v>
       </c>
@@ -2756,7 +2761,7 @@
       <c r="D27" s="48"/>
       <c r="E27" s="60"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28">
       <c r="A28" s="43" t="s">
         <v>12</v>
       </c>
@@ -2765,7 +2770,7 @@
       <c r="D28" s="45"/>
       <c r="E28" s="59"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29">
       <c r="A29" s="43" t="s">
         <v>12</v>
       </c>
@@ -2774,7 +2779,7 @@
       <c r="D29" s="48"/>
       <c r="E29" s="60"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30">
       <c r="A30" s="43" t="s">
         <v>12</v>
       </c>
@@ -2783,7 +2788,7 @@
       <c r="D30" s="51"/>
       <c r="E30" s="61"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31">
       <c r="A31" s="40" t="s">
         <v>13</v>
       </c>
@@ -2800,7 +2805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32">
       <c r="A32" s="40" t="s">
         <v>13</v>
       </c>
@@ -2809,7 +2814,7 @@
       <c r="D32" s="35"/>
       <c r="E32" s="57"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33">
       <c r="A33" s="40" t="s">
         <v>13</v>
       </c>
@@ -2818,7 +2823,7 @@
       <c r="D33" s="42"/>
       <c r="E33" s="56"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34">
       <c r="A34" s="40" t="s">
         <v>13</v>
       </c>
@@ -2827,7 +2832,7 @@
       <c r="D34" s="35"/>
       <c r="E34" s="57"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35">
       <c r="A35" s="40" t="s">
         <v>13</v>
       </c>
@@ -2836,7 +2841,7 @@
       <c r="D35" s="42"/>
       <c r="E35" s="56"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36">
       <c r="A36" s="40" t="s">
         <v>13</v>
       </c>
@@ -2857,21 +2862,21 @@
   <sheetPr/>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="12.75" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.8333333333333" defaultRowHeight="12.75" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="11.1666666666667" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
-    <col min="4" max="4" width="10.3333333333333" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="true"/>
+    <col min="2" max="2" width="11.166666666667" customWidth="true"/>
+    <col min="3" max="3" width="13.5" customWidth="true"/>
+    <col min="4" max="4" width="10.333333333333" customWidth="true"/>
+    <col min="6" max="6" width="13.5" customWidth="true"/>
+    <col min="8" max="8" width="14.5" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2885,7 +2890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2900,7 +2905,7 @@
       </c>
       <c r="E2" s="36"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
@@ -2914,7 +2919,7 @@
         <v>0.0007</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2931,7 +2936,7 @@
       <c r="G4" s="36"/>
       <c r="H4" s="37"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5">
       <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
@@ -2948,7 +2953,7 @@
       <c r="G5" s="36"/>
       <c r="H5" s="37"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6">
       <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
@@ -2964,7 +2969,7 @@
       <c r="G6" s="36"/>
       <c r="H6" s="37"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7">
       <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
@@ -2978,7 +2983,7 @@
         <v>0.004</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8">
       <c r="A8" s="20" t="s">
         <v>7</v>
       </c>
@@ -2992,7 +2997,7 @@
         <v>0.001</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -3006,7 +3011,7 @@
         <v>0.001</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -3020,7 +3025,7 @@
         <v>0.001</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11">
       <c r="A11" s="24" t="s">
         <v>7</v>
       </c>
@@ -3034,7 +3039,7 @@
         <v>0.001</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12">
       <c r="A12" s="20" t="s">
         <v>7</v>
       </c>
@@ -3048,7 +3053,7 @@
         <v>0.001</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13">
       <c r="A13" s="24" t="s">
         <v>7</v>
       </c>
@@ -3062,7 +3067,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14">
       <c r="A14" s="28" t="s">
         <v>6</v>
       </c>
@@ -3076,7 +3081,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15">
       <c r="A15" s="32" t="s">
         <v>6</v>
       </c>
@@ -3090,7 +3095,7 @@
         <v>0.005</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16">
       <c r="A16" s="28" t="s">
         <v>6</v>
       </c>
@@ -3104,7 +3109,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17">
       <c r="A17" s="28" t="s">
         <v>6</v>
       </c>
@@ -3122,4 +3127,105 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="true"/>
+    <col min="2" max="2" width="8.7109375" customWidth="true"/>
+    <col min="3" max="3" width="6.7109375" customWidth="true"/>
+    <col min="4" max="4" width="8.7109375" customWidth="true"/>
+    <col min="5" max="5" width="15.7109375" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="69" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1.5600000000000001</v>
+      </c>
+      <c r="B2">
+        <v>0.00078000000000000009</v>
+      </c>
+      <c r="C2">
+        <v>0.00020000000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.00098000000000000019</v>
+      </c>
+      <c r="E2">
+        <v>0.00062820512820512832</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="B3">
+        <v>0.039450000000000006</v>
+      </c>
+      <c r="C3">
+        <v>0.02</v>
+      </c>
+      <c r="D3">
+        <v>0.059450000000000003</v>
+      </c>
+      <c r="E3">
+        <v>0.00075348542458808618</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>81.230000000000004</v>
+      </c>
+      <c r="B4">
+        <v>0.040615000000000005</v>
+      </c>
+      <c r="C4">
+        <v>0.02</v>
+      </c>
+      <c r="D4">
+        <v>0.060615000000000002</v>
+      </c>
+      <c r="E4">
+        <v>0.00074621445278837866</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>100.67</v>
+      </c>
+      <c r="B5">
+        <v>0.050335000000000005</v>
+      </c>
+      <c r="C5">
+        <v>0.02</v>
+      </c>
+      <c r="D5">
+        <v>0.070335000000000009</v>
+      </c>
+      <c r="E5">
+        <v>0.00069866891824774027</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>